<commit_message>
20 cases completed for Aetna
</commit_message>
<xml_diff>
--- a/aetna/src/main/resources/AetnaProvidersPage_ExpectedElements.xlsx
+++ b/aetna/src/main/resources/AetnaProvidersPage_ExpectedElements.xlsx
@@ -3,23 +3,35 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamin\IdeaProjects\AutomationFramework_Team3\aetna\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E541961-6A2E-4566-B1DD-685A23CC8B93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F89436-B710-409C-A306-9716AA3929D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="providersPageTitle" sheetId="1" r:id="rId1"/>
     <sheet name="contactUsPageTitle" sheetId="2" r:id="rId2"/>
     <sheet name="spanishPageTitle" sheetId="3" r:id="rId3"/>
+    <sheet name="exploreMenuItems" sheetId="4" r:id="rId4"/>
+    <sheet name="claimsSubMenuCount" sheetId="5" r:id="rId5"/>
+    <sheet name="claimsSubMenuText" sheetId="6" r:id="rId6"/>
+    <sheet name="transcriptText" sheetId="7" r:id="rId7"/>
+    <sheet name="coronaVirusFcatTitle" sheetId="8" r:id="rId8"/>
+    <sheet name="quickLinksTabs" sheetId="9" r:id="rId9"/>
+    <sheet name="quickLinksCount" sheetId="10" r:id="rId10"/>
+    <sheet name="newsLetterTitle" sheetId="11" r:id="rId11"/>
+    <sheet name="exploreHealthCareTitle" sheetId="12" r:id="rId12"/>
+    <sheet name="helpfulLinksCount" sheetId="13" r:id="rId13"/>
+    <sheet name="helpfulLinksUrl" sheetId="14" r:id="rId14"/>
+    <sheet name="footerSectionLinks" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Aetna for Health Care Providers | Resources &amp; Support for Health Care Professionals</t>
   </si>
@@ -36,16 +48,125 @@
   </si>
   <si>
     <t>Aetna para proveedores del cuidado de salud | Recursos y apoyo para profesionales de la salud</t>
+  </si>
+  <si>
+    <t>Aetna.com</t>
+  </si>
+  <si>
+    <t>For Providers</t>
+  </si>
+  <si>
+    <t>For Employers</t>
+  </si>
+  <si>
+    <t>For Agents/Brokers</t>
+  </si>
+  <si>
+    <t>For Partners</t>
+  </si>
+  <si>
+    <t>Careers</t>
+  </si>
+  <si>
+    <t>About Us</t>
+  </si>
+  <si>
+    <t>Claims, payment &amp; reimbursement overview</t>
+  </si>
+  <si>
+    <t>Getting paid and submitting claims</t>
+  </si>
+  <si>
+    <t>Disputes and appeals</t>
+  </si>
+  <si>
+    <t>Fee schedules</t>
+  </si>
+  <si>
+    <t>Precertification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome to Aetna.com! Thank you for your interest in joining our Network. You can complete your request for participation here in a few easy steps
+  Once you complete your request, we will evaluate the current need to service our membership in your Area.
+  If we don’t intend to pursue a contract, we will notify you via email, please check your SPAM folder.
+  If we intend to pursue a contract, a local network manager will reach out to you to begin the contracting process, if required.
+  This contract is an electronic document that needs to be signed by you using the AdobeSign Process. Please sign and return the contract thru AdobeSign. 
+  If you do not see the email, please check your SPAM folder for this document.
+  Once Network receives your signed contract, they’ll request that the credentialing process gets started.
+  We use CAQH to obtain your credentialing application for most states.
+  If you’re located in Washington, if you’re a physician located in Arkansas or if you’re joining the
+  Allina Health | Aetna joint venture network in Minnesota, we use different vendors to obtain your credentialing data.
+  When using CAQH, ProviderSource/Medversant or any other Credentialing vendor, remember that you must designate Aetna as an authorized health plan to access your credentialing application.
+  Credentialing can take approximately 45 days to complete.
+  Once you have been approved in the credentialing process, Aetna will countersign and return your final contract via email through AdobeSign.
+  Aetna systems will be updated to reflect your participation effective date and Aetna members will be able to see your information in the directory.  You are now ready to submit claims.
+  Additionally, you will receive a welcome email with resources to help you in your journey.
+  Thank You for your interest in participating in our Networks!
+ </t>
+  </si>
+  <si>
+    <t>COVID-19 Resources &amp; Support for Aetna Providers</t>
+  </si>
+  <si>
+    <t>https://www.aetna.com/health-care-professionals/join-the-aetna-network.html</t>
+  </si>
+  <si>
+    <t>https://www.aetna.com/health-care-professionals/precertification/precertification-lists.html</t>
+  </si>
+  <si>
+    <t>https://www.aetna.com/health-care-professionals/medicare.html</t>
+  </si>
+  <si>
+    <t>https://www.aetna.com/health-care-professionals/clinical-policy-bulletins.html</t>
+  </si>
+  <si>
+    <t>OfficeLink Updates Newsletter Archive | Aetna</t>
+  </si>
+  <si>
+    <t>Provider Education &amp; Manuals – Health Care Professionals | Aetna</t>
+  </si>
+  <si>
+    <t>https://www.aetna.com/health-care-professionals/claims-payment-reimbursement.html</t>
+  </si>
+  <si>
+    <t>https://www.availity.com/</t>
+  </si>
+  <si>
+    <t>https://www.aetna.com/health-care-professionals/clinical-policy-bulletins/pharmacy-clinical-policy-bulletins.html</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/aetna/?hl=en</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/aetna</t>
+  </si>
+  <si>
+    <t>https://twitter.com/aetna</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/aetna</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/company/aetna</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -68,13 +189,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -369,6 +493,156 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{740BAC9E-44AA-4EA6-B237-C44D2DFAEF10}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F01CA6-E1D5-4796-B088-E4A9D74DC5D5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A057E92-C728-443E-95F4-2AF7EE4649F1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EEA8397-37DF-4492-AE6D-C7452B2E39A0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="40.1328125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B1C66DB-18D4-442A-8E13-31C69323EC2C}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6022C570-8EA6-4179-9D84-F147EF480220}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44E8DE30-235E-4CFD-AFE2-23FC1C47B07F}">
   <dimension ref="A1"/>
@@ -394,7 +668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F0F0C89-E817-4E56-B39F-84140B0647B3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -407,4 +681,199 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC8D9A2-9482-43B6-86F9-F695F0FE3CD2}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="19.86328125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15507A03-A5AD-49E7-9EAF-F39E8D642757}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A42C9F-DFDF-440C-9976-40A8594C6DA7}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="53.86328125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3505AB8A-59E1-4DCC-AC35-51C9F88DC16B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="155.33203125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21DE0B29-9634-4ED1-B8F2-797F1F992460}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC1DE41-15CC-4EAD-801F-EEF6FA3B2B96}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{393997E6-18ED-4151-9A93-F0BFCA4E6438}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{20400AB8-8F4F-48EB-B703-622EB6870D22}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{006D6248-5E88-4452-AA66-6E90DAE1AB44}"/>
+    <hyperlink ref="A1" r:id="rId4" xr:uid="{694884B0-CA00-45EC-8324-F322636C4D0F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>